<commit_message>
Fix bug in build_params, and now model seems equal to test with rng = 44
</commit_message>
<xml_diff>
--- a/app_main/Experiments/results/test/results.xlsx
+++ b/app_main/Experiments/results/test/results.xlsx
@@ -30,7 +30,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -48,11 +48,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -64,6 +68,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -142,7 +150,7 @@
   <cols>
     <col min="1" max="1" width="2.140625" customWidth="true"/>
     <col min="2" max="2" width="12.7109375" customWidth="true"/>
-    <col min="3" max="3" width="4.7109375" customWidth="true"/>
+    <col min="3" max="3" width="3.7109375" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
   </cols>
@@ -152,33 +160,33 @@
         <v>0</v>
       </c>
       <c r="B2" s="0">
-        <v>0.25869565217391305</v>
+        <v>0.27826086956521739</v>
       </c>
       <c r="C2" s="0">
-        <v>0.25</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="D2" s="0">
-        <v>0.52753623188405796</v>
+        <v>0.63478260869565217</v>
       </c>
       <c r="E2" s="0">
-        <v>0.13333333333333333</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0">
-        <v>0.25869565217391305</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C3" s="0">
-        <v>0.25</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="D3" s="0">
-        <v>0.52753623188405796</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E3" s="0">
-        <v>0.13333333333333333</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
experiments test for cnn
</commit_message>
<xml_diff>
--- a/app_main/Experiments/results/test/results.xlsx
+++ b/app_main/Experiments/results/test/results.xlsx
@@ -30,7 +30,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -52,11 +52,14 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -72,6 +75,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,7 +151,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E3"/>
+  <dimension ref="A2:E4"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.140625" customWidth="true"/>
@@ -157,19 +163,19 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>0.27826086956521739</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="C2" s="0">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.54492753623188395</v>
+      </c>
+      <c r="E2" s="0">
         <v>0.20000000000000001</v>
-      </c>
-      <c r="D2" s="0">
-        <v>0.63478260869565217</v>
-      </c>
-      <c r="E2" s="0">
-        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="3">
@@ -177,16 +183,33 @@
         <v>1</v>
       </c>
       <c r="B3" s="0">
-        <v>0.16666666666666666</v>
+        <v>0.13095238095238096</v>
       </c>
       <c r="C3" s="0">
         <v>0.10000000000000001</v>
       </c>
       <c r="D3" s="0">
-        <v>0.16666666666666666</v>
+        <v>0.61904761904761907</v>
       </c>
       <c r="E3" s="0">
-        <v>0.5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0">
+        <v>0.27826086956521739</v>
+      </c>
+      <c r="C4" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="D4" s="0">
+        <v>0.63478260869565217</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0.66666666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>